<commit_message>
looks like more to debug on heating season predictions
</commit_message>
<xml_diff>
--- a/A_prepost_processing/CAPITOUl_Whole_Year/Months_comparison.xlsx
+++ b/A_prepost_processing/CAPITOUl_Whole_Year/Months_comparison.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wulic\Documents\GitHub\VCWG_EP_Experiments\A_prepost_processing\CAPITOUl_Whole_Year\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6137DA-1E50-410F-A71B-5CCF86548E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="1" r:id="rId1"/>
     <sheet name="Prediction" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -101,8 +107,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,10 +160,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,7 +177,989 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Prediction!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensor_idx_NMBE_Percent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Prediction!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12_WithCooling</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11_WithoutCooling</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12_WithoutCooling</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Prediction!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.49</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.09</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.31</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.31</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2.27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-2.97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.82</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E21-4E01-94D5-EBA0D9461552}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2128372543"/>
+        <c:axId val="2128372959"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2128372543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2128372959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2128372959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2128372543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81526855-58D8-AD4B-5A6A-5A7DC4364555}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -211,7 +1205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,9 +1237,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -277,6 +1289,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,14 +1482,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,21 +1503,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2.35392931899449</v>
+        <v>2.3539293189944899</v>
       </c>
       <c r="C2">
-        <v>71.84940867706131</v>
+        <v>71.849408677061305</v>
       </c>
       <c r="D2">
-        <v>7.09415569143797</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>7.0941556914379698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -492,60 +1525,60 @@
         <v>3.818003445096982</v>
       </c>
       <c r="C3">
-        <v>44.79807753355708</v>
+        <v>44.798077533557077</v>
       </c>
       <c r="D3">
-        <v>0.5344055959131949</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.53440559591319492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>18.14609982552014</v>
+        <v>18.146099825520139</v>
       </c>
       <c r="C4">
-        <v>18.32341130314459</v>
+        <v>18.323411303144589</v>
       </c>
       <c r="D4">
-        <v>0.06956270325265428</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>6.9562703252654276E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>49.08209537107509</v>
+        <v>49.082095371075091</v>
       </c>
       <c r="C5">
-        <v>1.072252611201146</v>
+        <v>1.0722526112011459</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>57.41684716131331</v>
+        <v>57.416847161313306</v>
       </c>
       <c r="C6">
-        <v>0.4552247646494687</v>
+        <v>0.45522476464946871</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>58.39540190526943</v>
+        <v>58.395401905269431</v>
       </c>
       <c r="C7">
         <v>0.1601203380486925</v>
@@ -554,21 +1587,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>37.10472199360878</v>
+        <v>37.104721993608777</v>
       </c>
       <c r="C8">
-        <v>3.155207546477212</v>
+        <v>3.1552075464772118</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -576,32 +1609,32 @@
         <v>20.48790575555546</v>
       </c>
       <c r="C9">
-        <v>19.42667217750173</v>
+        <v>19.426672177501729</v>
       </c>
       <c r="D9">
-        <v>0.002332433406324095</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>2.3324334063240951E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.2484896404358171</v>
+        <v>0.24848964043581709</v>
       </c>
       <c r="C10">
         <v>94.30884732409244</v>
       </c>
       <c r="D10">
-        <v>8.464317058278587</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>8.4643170582785867</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.001098087251627208</v>
+        <v>1.098087251627208E-3</v>
       </c>
       <c r="C11">
         <v>105.9475752058796</v>
@@ -610,21 +1643,21 @@
         <v>15.65301076849043</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0.9825816297839802</v>
+        <v>0.98258162978398023</v>
       </c>
       <c r="C12">
-        <v>39.41528738360998</v>
+        <v>39.415287383609979</v>
       </c>
       <c r="D12">
-        <v>21.05793507366618</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>21.057935073666179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -632,27 +1665,27 @@
         <v>1.589313498430549</v>
       </c>
       <c r="C13">
-        <v>18.41817679707537</v>
+        <v>18.418176797075368</v>
       </c>
       <c r="D13">
-        <v>8.066318928511469</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>8.0663189285114694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>7.263410921655646</v>
+        <v>7.2634109216556464</v>
       </c>
       <c r="C14">
-        <v>5.931935072274057</v>
+        <v>5.9319350722740571</v>
       </c>
       <c r="D14">
-        <v>2.694961067765583</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>2.6949610677655831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -660,32 +1693,32 @@
         <v>17.41795242778705</v>
       </c>
       <c r="C15">
-        <v>0.05200867181348574</v>
+        <v>5.2008671813485743E-2</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>20.04747423585153</v>
+        <v>20.047474235851531</v>
       </c>
       <c r="C16">
-        <v>0.0003430523220072414</v>
+        <v>3.430523220072414E-4</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>20.10189674039283</v>
+        <v>20.101896740392831</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -694,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -702,41 +1735,41 @@
         <v>13.8812283610302</v>
       </c>
       <c r="C18">
-        <v>0.2425889547425883</v>
+        <v>0.24258895474258829</v>
       </c>
       <c r="D18">
-        <v>0.06275581416673547</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>6.2755814166735466E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>8.349374324765892</v>
+        <v>8.3493743247658916</v>
       </c>
       <c r="C19">
-        <v>5.014945362372321</v>
+        <v>5.0149453623723206</v>
       </c>
       <c r="D19">
         <v>1.518242001221753</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0.08653530363140446</v>
+        <v>8.6535303631404464E-2</v>
       </c>
       <c r="C20">
-        <v>60.23240721370732</v>
+        <v>60.232407213707319</v>
       </c>
       <c r="D20">
         <v>25.36755864902614</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -744,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>69.45848850407108</v>
+        <v>69.458488504071084</v>
       </c>
       <c r="D21">
         <v>34.82971442878123</v>
@@ -756,28 +1789,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" activeCellId="1" sqref="A1:A1048576 E1:E1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -794,7 +1832,7 @@
         <v>6.19</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -811,7 +1849,7 @@
         <v>-0.85</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -828,7 +1866,7 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -845,7 +1883,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -853,21 +1891,21 @@
         <v>6.5</v>
       </c>
       <c r="C6">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D6">
         <v>5.58</v>
       </c>
       <c r="E6">
-        <v>-2.28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>-2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>9.970000000000001</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="C7">
         <v>3.04</v>
@@ -879,12 +1917,12 @@
         <v>-3.49</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>8.449999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="C8">
         <v>4.12</v>
@@ -896,7 +1934,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -907,13 +1945,13 @@
         <v>3.26</v>
       </c>
       <c r="D9">
-        <v>8.460000000000001</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="E9">
         <v>-3.91</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -921,7 +1959,7 @@
         <v>16.72</v>
       </c>
       <c r="C10">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D10">
         <v>21.01</v>
@@ -930,7 +1968,7 @@
         <v>9.65</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -947,7 +1985,7 @@
         <v>12.59</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -964,7 +2002,7 @@
         <v>6.31</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -981,7 +2019,7 @@
         <v>-0.67</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -998,7 +2036,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1015,7 +2053,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1023,21 +2061,21 @@
         <v>6.5</v>
       </c>
       <c r="C16">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D16">
-        <v>4.81</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="E16">
         <v>-1.31</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>9.970000000000001</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="C17">
         <v>3.04</v>
@@ -1049,12 +2087,12 @@
         <v>-2.27</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18">
-        <v>8.449999999999999</v>
+        <v>8.4499999999999993</v>
       </c>
       <c r="C18">
         <v>4.12</v>
@@ -1066,7 +2104,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1083,7 +2121,7 @@
         <v>-2.97</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +2129,7 @@
         <v>16.72</v>
       </c>
       <c r="C20">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D20">
         <v>20.97</v>
@@ -1100,7 +2138,7 @@
         <v>9.82</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1119,5 +2157,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>